<commit_message>
Refactor funds layout component to utilize client-side rendering with useParams for dynamic metadata updates based on startupId. Implemented useEffect hooks to manage metadata state and document title updates.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/templates/accelerators-template.xlsx
+++ b/src/lib/scripts/seed-data/templates/accelerators-template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,6 +425,7 @@
     <col min="21" max="21" width="13.83203125" customWidth="1"/>
     <col min="22" max="22" width="11.83203125" customWidth="1"/>
     <col min="23" max="23" width="31.83203125" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -497,6 +498,9 @@
       <c r="W1" t="str">
         <v>notes</v>
       </c>
+      <c r="X1" t="str">
+        <v>visibility_level</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -568,10 +572,13 @@
       <c r="W2" t="str">
         <v>Rolling applications accepted</v>
       </c>
+      <c r="X2" t="str">
+        <v>PRO</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:W2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance data seeding scripts by updating type definitions to include Date and null values, improving data handling in bulk-seed and related functions.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/templates/accelerators-template.xlsx
+++ b/src/lib/scripts/seed-data/templates/accelerators-template.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="accelerators template" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="ValidationData" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
   <si>
     <t>name</t>
   </si>
@@ -86,19 +87,360 @@
   </si>
   <si>
     <t>visibility_level</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>in-person</t>
+  </si>
+  <si>
+    <t>3 months</t>
+  </si>
+  <si>
+    <t>1-10</t>
+  </si>
+  <si>
+    <t>Pre-seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- Tech
+    B2B SaaS</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>0-25K</t>
+  </si>
+  <si>
+    <t>&lt;1%</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>pitch_deck</t>
+  </si>
+  <si>
+    <t>FREE</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>remote</t>
+  </si>
+  <si>
+    <t>6 months</t>
+  </si>
+  <si>
+    <t>11-20</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Fintech</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>1-3%</t>
+  </si>
+  <si>
+    <t>25K-50K</t>
+  </si>
+  <si>
+    <t>1-5%</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>hybrid</t>
+  </si>
+  <si>
+    <t>12 months</t>
+  </si>
+  <si>
+    <t>21-50</t>
+  </si>
+  <si>
+    <t>Series A</t>
+  </si>
+  <si>
+    <t>Healthtech</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>4-6%</t>
+  </si>
+  <si>
+    <t>50K-100K</t>
+  </si>
+  <si>
+    <t>6-10%</t>
+  </si>
+  <si>
+    <t>comprehensive</t>
+  </si>
+  <si>
+    <t>financial_projections</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>51-100</t>
+  </si>
+  <si>
+    <t>Series B</t>
+  </si>
+  <si>
+    <t>AI/ML</t>
+  </si>
+  <si>
+    <t>LATAM</t>
+  </si>
+  <si>
+    <t>7-10%</t>
+  </si>
+  <si>
+    <t>100K-250K</t>
+  </si>
+  <si>
+    <t>11-20%</t>
+  </si>
+  <si>
+    <t>business_plan</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>100+</t>
+  </si>
+  <si>
+    <t>Series C</t>
+  </si>
+  <si>
+    <t>Deep tech</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>10%+</t>
+  </si>
+  <si>
+    <t>250K-500K</t>
+  </si>
+  <si>
+    <t>20%+</t>
+  </si>
+  <si>
+    <t>traction_data</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Climate tech</t>
+  </si>
+  <si>
+    <t>Western Europe</t>
+  </si>
+  <si>
+    <t>500K+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Eastern Europe</t>
+  </si>
+  <si>
+    <t>E-commerce</t>
+  </si>
+  <si>
+    <t>Continental Europe</t>
+  </si>
+  <si>
+    <t>Marketplace</t>
+  </si>
+  <si>
+    <t>Middle East</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Web3</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Developer tools</t>
+  </si>
+  <si>
+    <t>East Asia</t>
+  </si>
+  <si>
+    <t>Cybersecurity</t>
+  </si>
+  <si>
+    <t>South Asia</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>South East Asia</t>
+  </si>
+  <si>
+    <t>AdTech</t>
+  </si>
+  <si>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>PropTech</t>
+  </si>
+  <si>
+    <t>EMEA</t>
+  </si>
+  <si>
+    <t>InsurTech</t>
+  </si>
+  <si>
+    <t>Emerging Markets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- Non-Tech / Other
+    Agriculture</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>Biotechnology</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Consumer Goods</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Environmental Services</t>
+  </si>
+  <si>
+    <t>Fashion</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Healthcare Services</t>
+  </si>
+  <si>
+    <t>Hospitality</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Non-profit</t>
+  </si>
+  <si>
+    <t>Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>Telecommunications</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,8 +463,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,80 +811,80 @@
     <col min="1" max="25" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1546,90 +1889,526 @@
     <row r="1000" spans="5:25" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="26">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="E10:E1000">
-      <formula1>"form,email,other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="E2:E1000">
-      <formula1>"form,email,other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="F10:F1000">
-      <formula1>"in-person,remote,hybrid"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="F2:F1000">
-      <formula1>"in-person,remote,hybrid"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="G10:G1000">
-      <formula1>"3 months,6 months,12 months,ongoing,variable"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="G2:G1000">
-      <formula1>"3 months,6 months,12 months,ongoing,variable"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="J10:J1000">
-      <formula1>"1-10,11-20,21-50,51-100,100+"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="J2:J1000">
-      <formula1>"1-10,11-20,21-50,51-100,100+"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="M10:M1000">
-      <formula1>"Pre-seed,Seed,Series A,Series B,Series C,Growth,All"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="M2:M1000">
-      <formula1>"Pre-seed,Seed,Series A,Series B,Series C,Growth,All"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="N10:N1000">
-      <formula1>"-- Tech
-    B2B SaaS,Fintech,Healthtech,AI/ML,Deep tech,Climate tech,Consumer,E-commerce,Marketplace,Gaming,Web3,Developer tools,Cybersecurity,Logistics,AdTech,PropTech,InsurTech,-- Non-Tech / Other
-    Agriculture,Automotive,Biotechnology,Construction,Consulting,Consumer Goods,Education,Energy,Entertainment,Environmental Services,Fashion,Food &amp; Beverage,Government,Healthcare Services,Hospitality,Human Resources,Insurance,Legal,Manufacturing,Media,Non-profit,Pharmaceuticals,Real Estate,Retail,Telecommunications,Transportation,Utilities,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="N2:N1000">
-      <formula1>"-- Tech
-    B2B SaaS,Fintech,Healthtech,AI/ML,Deep tech,Climate tech,Consumer,E-commerce,Marketplace,Gaming,Web3,Developer tools,Cybersecurity,Logistics,AdTech,PropTech,InsurTech,-- Non-Tech / Other
-    Agriculture,Automotive,Biotechnology,Construction,Consulting,Consumer Goods,Education,Energy,Entertainment,Environmental Services,Fashion,Food &amp; Beverage,Government,Healthcare Services,Hospitality,Human Resources,Insurance,Legal,Manufacturing,Media,Non-profit,Pharmaceuticals,Real Estate,Retail,Telecommunications,Transportation,Utilities,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="O10:O1000">
-      <formula1>"Global,North America,South America,LATAM,Europe,Western Europe,Eastern Europe,Continental Europe,Middle East,Africa,Asia,East Asia,South Asia,South East Asia,Oceania,EMEA,Emerging Markets"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="O2:O1000">
-      <formula1>"Global,North America,South America,LATAM,Europe,Western Europe,Eastern Europe,Continental Europe,Middle East,Africa,Asia,East Asia,South Asia,South East Asia,Oceania,EMEA,Emerging Markets"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="P10:P1000">
-      <formula1>"0%,1-3%,4-6%,7-10%,10%+,variable"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="P2:P1000">
-      <formula1>"0%,1-3%,4-6%,7-10%,10%+,variable"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="Q10:Q1000">
-      <formula1>"0-25K,25K-50K,50K-100K,100K-250K,250K-500K,500K+"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="Q2:Q1000">
-      <formula1>"0-25K,25K-50K,50K-100K,100K-250K,250K-500K,500K+"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="R10:R1000">
-      <formula1>"&lt;1%,1-5%,6-10%,11-20%,20%+"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="R2:R1000">
-      <formula1>"&lt;1%,1-5%,6-10%,11-20%,20%+"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="S10:S1000">
-      <formula1>"simple,standard,comprehensive"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="S2:S1000">
-      <formula1>"simple,standard,comprehensive"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="T10:T1000">
-      <formula1>"pitch_deck,video,financial_projections,business_plan,traction_data"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="T2:T1000">
-      <formula1>"pitch_deck,video,financial_projections,business_plan,traction_data"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="Y10:Y1000">
-      <formula1>"FREE,PRO,MAX"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the list. For multiple values, enter them as a comma-separated list." sqref="Y2:Y1000">
-      <formula1>"FREE,PRO,MAX"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="E10:E1000">
+      <formula1>ValidationData!$E$1:$E$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="E2:E1000">
+      <formula1>ValidationData!$E$1:$E$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="F10:F1000">
+      <formula1>ValidationData!$F$1:$F$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="F2:F1000">
+      <formula1>ValidationData!$F$1:$F$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="G10:G1000">
+      <formula1>ValidationData!$G$1:$G$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="G2:G1000">
+      <formula1>ValidationData!$G$1:$G$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="J10:J1000">
+      <formula1>ValidationData!$J$1:$J$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="J2:J1000">
+      <formula1>ValidationData!$J$1:$J$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="M10:M1000">
+      <formula1>ValidationData!$M$1:$M$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="M2:M1000">
+      <formula1>ValidationData!$M$1:$M$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="N10:N1000">
+      <formula1>ValidationData!$N$1:$N$45</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="N2:N1000">
+      <formula1>ValidationData!$N$1:$N$45</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="O10:O1000">
+      <formula1>ValidationData!$O$1:$O$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="O2:O1000">
+      <formula1>ValidationData!$O$1:$O$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="P10:P1000">
+      <formula1>ValidationData!$P$1:$P$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="P2:P1000">
+      <formula1>ValidationData!$P$1:$P$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Q10:Q1000">
+      <formula1>ValidationData!$Q$1:$Q$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Q2:Q1000">
+      <formula1>ValidationData!$Q$1:$Q$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="R10:R1000">
+      <formula1>ValidationData!$R$1:$R$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="R2:R1000">
+      <formula1>ValidationData!$R$1:$R$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="S10:S1000">
+      <formula1>ValidationData!$S$1:$S$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="S2:S1000">
+      <formula1>ValidationData!$S$1:$S$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="T10:T1000">
+      <formula1>ValidationData!$T$1:$T$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="T2:T1000">
+      <formula1>ValidationData!$T$1:$T$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Y10:Y1000">
+      <formula1>ValidationData!$Y$1:$Y$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Y2:Y1000">
+      <formula1>ValidationData!$Y$1:$Y$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E1:Y45"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>70</v>
+      </c>
+      <c r="R4" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O5" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>79</v>
+      </c>
+      <c r="R5" t="s">
+        <v>80</v>
+      </c>
+      <c r="T5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>82</v>
+      </c>
+      <c r="N6" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" t="s">
+        <v>84</v>
+      </c>
+      <c r="P6" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>93</v>
+      </c>
+      <c r="O10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>95</v>
+      </c>
+      <c r="O11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>97</v>
+      </c>
+      <c r="O12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>99</v>
+      </c>
+      <c r="O13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>101</v>
+      </c>
+      <c r="O14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>103</v>
+      </c>
+      <c r="O15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>105</v>
+      </c>
+      <c r="O16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>107</v>
+      </c>
+      <c r="O17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove obsolete Excel files for data seeding and update templates for accelerators, angels, and targets with new array key handling in sheet-utils.ts.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/templates/accelerators-template.xlsx
+++ b/src/lib/scripts/seed-data/templates/accelerators-template.xlsx
@@ -104,8 +104,7 @@
     <t>Pre-seed</t>
   </si>
   <si>
-    <t xml:space="preserve">-- Tech
-    B2B SaaS</t>
+    <t>B2B SaaS</t>
   </si>
   <si>
     <t>Global</t>
@@ -342,8 +341,7 @@
     <t>Emerging Markets</t>
   </si>
   <si>
-    <t xml:space="preserve">-- Non-Tech / Other
-    Agriculture</t>
+    <t>Agriculture</t>
   </si>
   <si>
     <t>Automotive</t>
@@ -1889,82 +1887,82 @@
     <row r="1000" spans="5:25" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="26">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="E10:E1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="E10:E1000">
       <formula1>ValidationData!$E$1:$E$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="E2:E1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="E2:E1000">
       <formula1>ValidationData!$E$1:$E$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="F10:F1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="F10:F1000">
       <formula1>ValidationData!$F$1:$F$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="F2:F1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="F2:F1000">
       <formula1>ValidationData!$F$1:$F$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="G10:G1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="G10:G1000">
       <formula1>ValidationData!$G$1:$G$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="G2:G1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="G2:G1000">
       <formula1>ValidationData!$G$1:$G$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="J10:J1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="J10:J1000">
       <formula1>ValidationData!$J$1:$J$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="J2:J1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="J2:J1000">
       <formula1>ValidationData!$J$1:$J$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="M10:M1000">
+    <dataValidation type="list" allowBlank="1" errorStyle="information" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." sqref="M10:M1000">
       <formula1>ValidationData!$M$1:$M$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="M2:M1000">
+    <dataValidation type="list" allowBlank="1" errorStyle="information" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." sqref="M2:M1000">
       <formula1>ValidationData!$M$1:$M$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="N10:N1000">
+    <dataValidation type="list" allowBlank="1" errorStyle="information" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." sqref="N10:N1000">
       <formula1>ValidationData!$N$1:$N$45</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="N2:N1000">
+    <dataValidation type="list" allowBlank="1" errorStyle="information" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." sqref="N2:N1000">
       <formula1>ValidationData!$N$1:$N$45</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="O10:O1000">
+    <dataValidation type="list" allowBlank="1" errorStyle="information" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." sqref="O10:O1000">
       <formula1>ValidationData!$O$1:$O$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="O2:O1000">
+    <dataValidation type="list" allowBlank="1" errorStyle="information" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." sqref="O2:O1000">
       <formula1>ValidationData!$O$1:$O$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="P10:P1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="P10:P1000">
       <formula1>ValidationData!$P$1:$P$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="P2:P1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="P2:P1000">
       <formula1>ValidationData!$P$1:$P$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Q10:Q1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Q10:Q1000">
       <formula1>ValidationData!$Q$1:$Q$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Q2:Q1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Q2:Q1000">
       <formula1>ValidationData!$Q$1:$Q$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="R10:R1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="R10:R1000">
       <formula1>ValidationData!$R$1:$R$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="R2:R1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="R2:R1000">
       <formula1>ValidationData!$R$1:$R$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="S10:S1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="S10:S1000">
       <formula1>ValidationData!$S$1:$S$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="S2:S1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="S2:S1000">
       <formula1>ValidationData!$S$1:$S$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="T10:T1000">
+    <dataValidation type="list" allowBlank="1" errorStyle="information" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." sqref="T10:T1000">
       <formula1>ValidationData!$T$1:$T$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="T2:T1000">
+    <dataValidation type="list" allowBlank="1" errorStyle="information" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." sqref="T2:T1000">
       <formula1>ValidationData!$T$1:$T$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Y10:Y1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Y10:Y1000">
       <formula1>ValidationData!$Y$1:$Y$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Y2:Y1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Value" error="Please select a value from the dropdown list." sqref="Y2:Y1000">
       <formula1>ValidationData!$Y$1:$Y$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
feat: Remove obsolete seed data files for accelerators, angels, and targets; update templates for accelerators, angels, and targets; enhance ENUM value handling in db-utils and sheet-utils for better synchronization with SQL schema.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/templates/accelerators-template.xlsx
+++ b/src/lib/scripts/seed-data/templates/accelerators-template.xlsx
@@ -79,12 +79,14 @@
       <text>
         <r>
           <t xml:space="preserve">Possible values:
-- B2B SaaS
+- Software
 - Fintech
-- Healthtech
-- AI/ML
+- Healthcare
+- Medtech
+- AI
+- Computing
 - Deep tech
-- Climate tech
+- Climate
 - Consumer
 - E-commerce
 - Marketplace
@@ -93,36 +95,41 @@
 - Developer tools
 - Cybersecurity
 - Logistics
-- AdTech
-- PropTech
-- InsurTech
+- Adtech
+- Proptech
 - Agriculture
 - Automotive
 - Biotechnology
 - Construction
-- Consulting
-- Consumer Goods
 - Education
 - Energy
 - Entertainment
-- Environmental Services
+- Environment
 - Fashion
-- Food &amp; Beverage
+- Real estate
+- Food
+- IoT
 - Government
-- Healthcare Services
 - Hospitality
-- Human Resources
+- HR
 - Insurance
+- Security
+- Social
+- Aerospace
+- AR/VR
+- Mining
+- Advanced Materials
+- Biofuels
+- Hardware
+- Nanotechnology
 - Legal
 - Manufacturing
 - Media
-- Non-profit
 - Pharmaceuticals
-- Real Estate
 - Retail
 - Telecommunications
 - Transportation
-- Utilities
+- Agnostic
 - Other</t>
         </r>
       </text>
@@ -136,18 +143,32 @@
 - South America
 - LATAM
 - Europe
-- Western Europe
-- Eastern Europe
-- Continental Europe
 - Middle East
 - Africa
 - Asia
 - East Asia
+- South East Asia
 - South Asia
-- South East Asia
 - Oceania
 - EMEA
-- Emerging Markets</t>
+- Emerging Markets
+- India
+- China
+- Japan
+- Korea
+- Australia
+- United States
+- Canada
+- UK
+- France
+- Nigeria
+- Kenya
+- Egypt
+- Senegal
+- South Africa
+- Netherlands
+- Sweden
+- Other</t>
         </r>
       </text>
     </comment>
@@ -205,9 +226,8 @@
           <t xml:space="preserve">Possible values:
 - pitch_deck
 - video
-- financial_projections
-- business_plan
-- traction_data</t>
+- financials
+- business_plan</t>
         </r>
       </text>
     </comment>
@@ -216,6 +236,7 @@
         <r>
           <t xml:space="preserve">Possible values:
 - contact
+- airtable
 - typeform
 - google
 - generic</t>
@@ -239,7 +260,8 @@
           <t xml:space="preserve">Possible values:
 - FREE
 - PRO
-- MAX</t>
+- MAX
+- ENTERPRISE</t>
         </r>
       </text>
     </comment>
@@ -248,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="168">
   <si>
     <t>name</t>
   </si>
@@ -346,7 +368,7 @@
     <t>Pre-seed</t>
   </si>
   <si>
-    <t>B2B SaaS</t>
+    <t>Software</t>
   </si>
   <si>
     <t>Global</t>
@@ -412,252 +434,324 @@
     <t>video</t>
   </si>
   <si>
+    <t>airtable</t>
+  </si>
+  <si>
+    <t>browser_base</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>hybrid</t>
+  </si>
+  <si>
+    <t>12 months</t>
+  </si>
+  <si>
+    <t>21-50</t>
+  </si>
+  <si>
+    <t>Series A</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>4-6%</t>
+  </si>
+  <si>
+    <t>50K-100K</t>
+  </si>
+  <si>
+    <t>6-10%</t>
+  </si>
+  <si>
+    <t>comprehensive</t>
+  </si>
+  <si>
+    <t>financials</t>
+  </si>
+  <si>
     <t>typeform</t>
   </si>
   <si>
-    <t>browser_base</t>
-  </si>
-  <si>
-    <t>PRO</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>hybrid</t>
-  </si>
-  <si>
-    <t>12 months</t>
-  </si>
-  <si>
-    <t>21-50</t>
-  </si>
-  <si>
-    <t>Series A</t>
-  </si>
-  <si>
-    <t>Healthtech</t>
-  </si>
-  <si>
-    <t>South America</t>
-  </si>
-  <si>
-    <t>4-6%</t>
-  </si>
-  <si>
-    <t>50K-100K</t>
-  </si>
-  <si>
-    <t>6-10%</t>
-  </si>
-  <si>
-    <t>comprehensive</t>
-  </si>
-  <si>
-    <t>financial_projections</t>
+    <t>computer_use</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>51-100</t>
+  </si>
+  <si>
+    <t>Series B</t>
+  </si>
+  <si>
+    <t>Medtech</t>
+  </si>
+  <si>
+    <t>LATAM</t>
+  </si>
+  <si>
+    <t>7-10%</t>
+  </si>
+  <si>
+    <t>100K-250K</t>
+  </si>
+  <si>
+    <t>11-20%</t>
+  </si>
+  <si>
+    <t>business_plan</t>
   </si>
   <si>
     <t>google</t>
   </si>
   <si>
-    <t>computer_use</t>
-  </si>
-  <si>
-    <t>MAX</t>
-  </si>
-  <si>
-    <t>ongoing</t>
-  </si>
-  <si>
-    <t>51-100</t>
-  </si>
-  <si>
-    <t>Series B</t>
-  </si>
-  <si>
-    <t>AI/ML</t>
-  </si>
-  <si>
-    <t>LATAM</t>
-  </si>
-  <si>
-    <t>7-10%</t>
-  </si>
-  <si>
-    <t>100K-250K</t>
-  </si>
-  <si>
-    <t>11-20%</t>
-  </si>
-  <si>
-    <t>business_plan</t>
+    <t>hyperbrowser</t>
+  </si>
+  <si>
+    <t>ENTERPRISE</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>100+</t>
+  </si>
+  <si>
+    <t>Series C</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>10%+</t>
+  </si>
+  <si>
+    <t>250K-500K</t>
+  </si>
+  <si>
+    <t>20%+</t>
   </si>
   <si>
     <t>generic</t>
   </si>
   <si>
-    <t>hyperbrowser</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>100+</t>
-  </si>
-  <si>
-    <t>Series C</t>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Computing</t>
+  </si>
+  <si>
+    <t>Middle East</t>
+  </si>
+  <si>
+    <t>500K+</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
   <si>
     <t>Deep tech</t>
   </si>
   <si>
-    <t>Europe</t>
-  </si>
-  <si>
-    <t>10%+</t>
-  </si>
-  <si>
-    <t>250K-500K</t>
-  </si>
-  <si>
-    <t>20%+</t>
-  </si>
-  <si>
-    <t>traction_data</t>
-  </si>
-  <si>
-    <t>Growth</t>
-  </si>
-  <si>
-    <t>Climate tech</t>
-  </si>
-  <si>
-    <t>Western Europe</t>
-  </si>
-  <si>
-    <t>500K+</t>
-  </si>
-  <si>
-    <t>All</t>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Asia</t>
   </si>
   <si>
     <t>Consumer</t>
   </si>
   <si>
-    <t>Eastern Europe</t>
+    <t>East Asia</t>
   </si>
   <si>
     <t>E-commerce</t>
   </si>
   <si>
-    <t>Continental Europe</t>
+    <t>South East Asia</t>
   </si>
   <si>
     <t>Marketplace</t>
   </si>
   <si>
-    <t>Middle East</t>
+    <t>South Asia</t>
   </si>
   <si>
     <t>Gaming</t>
   </si>
   <si>
-    <t>Africa</t>
+    <t>Oceania</t>
   </si>
   <si>
     <t>Web3</t>
   </si>
   <si>
-    <t>Asia</t>
+    <t>EMEA</t>
   </si>
   <si>
     <t>Developer tools</t>
   </si>
   <si>
-    <t>East Asia</t>
+    <t>Emerging Markets</t>
   </si>
   <si>
     <t>Cybersecurity</t>
   </si>
   <si>
-    <t>South Asia</t>
+    <t>India</t>
   </si>
   <si>
     <t>Logistics</t>
   </si>
   <si>
-    <t>South East Asia</t>
-  </si>
-  <si>
-    <t>AdTech</t>
-  </si>
-  <si>
-    <t>Oceania</t>
-  </si>
-  <si>
-    <t>PropTech</t>
-  </si>
-  <si>
-    <t>EMEA</t>
-  </si>
-  <si>
-    <t>InsurTech</t>
-  </si>
-  <si>
-    <t>Emerging Markets</t>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Adtech</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Proptech</t>
+  </si>
+  <si>
+    <t>Korea</t>
   </si>
   <si>
     <t>Agriculture</t>
   </si>
   <si>
+    <t>Australia</t>
+  </si>
+  <si>
     <t>Automotive</t>
   </si>
   <si>
+    <t>United States</t>
+  </si>
+  <si>
     <t>Biotechnology</t>
   </si>
   <si>
+    <t>Canada</t>
+  </si>
+  <si>
     <t>Construction</t>
   </si>
   <si>
-    <t>Consulting</t>
-  </si>
-  <si>
-    <t>Consumer Goods</t>
+    <t>UK</t>
   </si>
   <si>
     <t>Education</t>
   </si>
   <si>
+    <t>France</t>
+  </si>
+  <si>
     <t>Energy</t>
   </si>
   <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
     <t>Entertainment</t>
   </si>
   <si>
-    <t>Environmental Services</t>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Egypt</t>
   </si>
   <si>
     <t>Fashion</t>
   </si>
   <si>
-    <t>Food &amp; Beverage</t>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Real estate</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>Sweden</t>
   </si>
   <si>
     <t>Government</t>
   </si>
   <si>
-    <t>Healthcare Services</t>
+    <t>Other</t>
   </si>
   <si>
     <t>Hospitality</t>
   </si>
   <si>
-    <t>Human Resources</t>
+    <t>HR</t>
   </si>
   <si>
     <t>Insurance</t>
   </si>
   <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Aerospace</t>
+  </si>
+  <si>
+    <t>AR/VR</t>
+  </si>
+  <si>
+    <t>Mining</t>
+  </si>
+  <si>
+    <t>Advanced Materials</t>
+  </si>
+  <si>
+    <t>Biofuels</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Nanotechnology</t>
+  </si>
+  <si>
     <t>Legal</t>
   </si>
   <si>
@@ -667,15 +761,9 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Non-profit</t>
-  </si>
-  <si>
     <t>Pharmaceuticals</t>
   </si>
   <si>
-    <t>Real Estate</t>
-  </si>
-  <si>
     <t>Retail</t>
   </si>
   <si>
@@ -685,10 +773,7 @@
     <t>Transportation</t>
   </si>
   <si>
-    <t>Utilities</t>
-  </si>
-  <si>
-    <t>Other</t>
+    <t>Agnostic</t>
   </si>
 </sst>
 </file>
@@ -2160,10 +2245,10 @@
   </sheetData>
   <dataValidations count="30">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="AA10:AA1000">
-      <formula1>ValidationData!$AA$1:$AA$3</formula1>
+      <formula1>ValidationData!$AA$1:$AA$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="AA2:AA1000">
-      <formula1>ValidationData!$AA$1:$AA$3</formula1>
+      <formula1>ValidationData!$AA$1:$AA$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="E10:E1000">
       <formula1>ValidationData!$E$1:$E$3</formula1>
@@ -2196,16 +2281,16 @@
       <formula1>ValidationData!$M$1:$M$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="N10:N1000">
-      <formula1>ValidationData!$N$1:$N$45</formula1>
+      <formula1>ValidationData!$N$1:$N$52</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="N2:N1000">
-      <formula1>ValidationData!$N$1:$N$45</formula1>
+      <formula1>ValidationData!$N$1:$N$52</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="O10:O1000">
-      <formula1>ValidationData!$O$1:$O$17</formula1>
+      <formula1>ValidationData!$O$1:$O$31</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="O2:O1000">
-      <formula1>ValidationData!$O$1:$O$17</formula1>
+      <formula1>ValidationData!$O$1:$O$31</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="P10:P1000">
       <formula1>ValidationData!$P$1:$P$6</formula1>
@@ -2232,16 +2317,16 @@
       <formula1>ValidationData!$S$1:$S$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="T10:T1000">
-      <formula1>ValidationData!$T$1:$T$5</formula1>
+      <formula1>ValidationData!$T$1:$T$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="T2:T1000">
-      <formula1>ValidationData!$T$1:$T$5</formula1>
+      <formula1>ValidationData!$T$1:$T$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="Y10:Y1000">
-      <formula1>ValidationData!$Y$1:$Y$4</formula1>
+      <formula1>ValidationData!$Y$1:$Y$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="Y2:Y1000">
-      <formula1>ValidationData!$Y$1:$Y$4</formula1>
+      <formula1>ValidationData!$Y$1:$Y$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="Z10:Z1000">
       <formula1>ValidationData!$Z$1:$Z$4</formula1>
@@ -2258,7 +2343,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:AA45"/>
+  <dimension ref="E1:AA52"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="5:27" x14ac:dyDescent="0.25">
@@ -2402,7 +2487,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:27" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>72</v>
       </c>
@@ -2436,282 +2521,362 @@
       <c r="Z4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="AA4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="7:25" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T5" t="s">
         <v>91</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="O11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="O14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="O17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="14:14" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="14:14" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="O18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="14:14" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="O19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="O20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="14:14" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="O21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="14:14" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="O22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="14:14" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="O23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N24" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="14:14" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="O24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="14:14" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="O25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N26" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="14:14" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="O26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="14:14" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="O27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="14:14" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="O28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="14:14" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="O29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="14:14" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="O30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
-        <v>132</v>
+        <v>146</v>
+      </c>
+      <c r="O31" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N34" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N35" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N36" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N37" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N38" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N39" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N40" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N41" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N42" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N43" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N44" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N45" t="s">
-        <v>146</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N51" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N52" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>